<commit_message>
edit teacher personal information
</commit_message>
<xml_diff>
--- a/database.xlsx
+++ b/database.xlsx
@@ -8,22 +8,23 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\code_gym\nga-nguyen\pet-project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8DAD7D40-8A08-4BE3-81F6-B1CB30D1C726}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6093449-62F3-460F-B031-90351CF0E64B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" activeTab="4" xr2:uid="{531ADD29-FA2D-43B7-9AD7-6F46602D30F8}"/>
+    <workbookView xWindow="4230" yWindow="2650" windowWidth="20930" windowHeight="9600" activeTab="1" xr2:uid="{531ADD29-FA2D-43B7-9AD7-6F46602D30F8}"/>
   </bookViews>
   <sheets>
     <sheet name="Teacher" sheetId="1" r:id="rId1"/>
-    <sheet name="Class" sheetId="5" r:id="rId2"/>
-    <sheet name="Student" sheetId="6" r:id="rId3"/>
-    <sheet name="Subject" sheetId="7" r:id="rId4"/>
-    <sheet name="Period" sheetId="9" r:id="rId5"/>
-    <sheet name="Timetable_period" sheetId="11" r:id="rId6"/>
-    <sheet name="Subject Teacher Record" sheetId="10" r:id="rId7"/>
-    <sheet name="Timetable" sheetId="8" r:id="rId8"/>
-    <sheet name="Faculty" sheetId="2" r:id="rId9"/>
-    <sheet name="Ethnicity" sheetId="4" r:id="rId10"/>
-    <sheet name="City" sheetId="3" r:id="rId11"/>
+    <sheet name="User" sheetId="12" r:id="rId2"/>
+    <sheet name="Class" sheetId="5" r:id="rId3"/>
+    <sheet name="Student" sheetId="6" r:id="rId4"/>
+    <sheet name="Subject" sheetId="7" r:id="rId5"/>
+    <sheet name="Period" sheetId="9" r:id="rId6"/>
+    <sheet name="Timetable_period" sheetId="11" r:id="rId7"/>
+    <sheet name="Subject Teacher Record" sheetId="10" r:id="rId8"/>
+    <sheet name="Timetable" sheetId="8" r:id="rId9"/>
+    <sheet name="Faculty" sheetId="2" r:id="rId10"/>
+    <sheet name="Ethnicity" sheetId="4" r:id="rId11"/>
+    <sheet name="City" sheetId="3" r:id="rId12"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -45,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1969" uniqueCount="997">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2003" uniqueCount="1015">
   <si>
     <t>id</t>
   </si>
@@ -3136,6 +3137,60 @@
   </si>
   <si>
     <t>periods_id</t>
+  </si>
+  <si>
+    <t>username</t>
+  </si>
+  <si>
+    <t>password</t>
+  </si>
+  <si>
+    <t>$2a$10$VbSCATiCKwPMQyl8agMCS.4xUGU125j5s7HK7Q4Ne1aNgwyO/7CDa</t>
+  </si>
+  <si>
+    <t>$2a$10$V7ReSrXYGWsLqMMS.oyP4OTNnUvDqVlScE.0bo.wzoUdJrhysTyOa</t>
+  </si>
+  <si>
+    <t>$2a$10$q9unEkjSA/io5v/Xah4chO57wKtaNHkQX7n3av.5c8LWuwHPXrndm</t>
+  </si>
+  <si>
+    <t>$2a$10$G7eEHVK.VfinZ5MKesg2j.qAtbR19VGuHOewXaOQhR3Ttz5Z9RXy6</t>
+  </si>
+  <si>
+    <t>$2a$10$3xOcp8Te31DnhFd.yrJnQ.NoxtpRqPAa9jbFuIStWBPCe9UT46oTW</t>
+  </si>
+  <si>
+    <t>$2a$10$1cy.UHw/5kfLA0mDIjiWC.BtmaNHpr9BaTi2kzRIgauCdqL4Nl2W6</t>
+  </si>
+  <si>
+    <t>$2a$10$5Y9/e1/.YMIFyuaxT6e1DeFmEziX8BI8tqYayPiCnIMzCMIaTIzJG</t>
+  </si>
+  <si>
+    <t>$2a$10$9GT5YLgO1zolRqNU566MNOgEQoIsrlu1oIv3r0wshcmXc5qerxUMy</t>
+  </si>
+  <si>
+    <t>$2a$10$/1KSvYnJN0O/5XRt/TAbLenvx4o311o9vyLb7tJc1TnuH9MzVQaOa</t>
+  </si>
+  <si>
+    <t>$2a$10$NAxxnaE0F1C9imkpo2yBPOepaODC/atuJpPJd35xXKwV/Lk/1oWxS</t>
+  </si>
+  <si>
+    <t>$2a$10$hkYN9599NGGzdZEqXW.WpOPg2NaQk9P2pRQqk2fr7r3SAu6oPFFr2</t>
+  </si>
+  <si>
+    <t>$2a$10$A2l1YscpbwhQ8knrhvk22.LwmUc./zG3ime8f4iSvM6622CSKLBta</t>
+  </si>
+  <si>
+    <t>$2a$10$fvcvbDw8DwIP4Lz8tC454.ckhlU15jy8T4pwgi3CaCggOiKSqcwfK</t>
+  </si>
+  <si>
+    <t>$2a$10$40J5NPf37shjTumah8q39eB.aXaAKMOvsKpeB1grMMrAVrpVtIusa</t>
+  </si>
+  <si>
+    <t>$2a$10$ZHavZpaEV7RfknMFsrVG2u9TkcSBg8bHw2eKynsTo3LvmMdvPskdW</t>
+  </si>
+  <si>
+    <t>user_id</t>
   </si>
 </sst>
 </file>
@@ -3593,10 +3648,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B2E27D4D-5B27-41C4-B9C0-1A3758213F19}">
-  <dimension ref="A1:K16"/>
+  <dimension ref="A1:L16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C36" sqref="C36"/>
+      <selection activeCell="B1" sqref="B1:L16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3609,7 +3664,7 @@
     <col min="10" max="10" width="25.7265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -3643,8 +3698,11 @@
       <c r="K1" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L1" t="s">
+        <v>1014</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>1</v>
       </c>
@@ -3678,8 +3736,11 @@
       <c r="K2">
         <v>2</v>
       </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.35">
       <c r="B3" t="s">
         <v>106</v>
       </c>
@@ -3710,8 +3771,11 @@
       <c r="K3">
         <v>4</v>
       </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.35">
       <c r="B4" t="s">
         <v>110</v>
       </c>
@@ -3742,8 +3806,11 @@
       <c r="K4">
         <v>1</v>
       </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.35">
       <c r="B5" t="s">
         <v>113</v>
       </c>
@@ -3774,8 +3841,11 @@
       <c r="K5">
         <v>2</v>
       </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L5">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.35">
       <c r="B6" t="s">
         <v>116</v>
       </c>
@@ -3806,8 +3876,11 @@
       <c r="K6">
         <v>1</v>
       </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L6">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.35">
       <c r="B7" t="s">
         <v>120</v>
       </c>
@@ -3838,8 +3911,11 @@
       <c r="K7">
         <v>3</v>
       </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L7">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>2</v>
       </c>
@@ -3873,8 +3949,11 @@
       <c r="K8">
         <v>2</v>
       </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L8">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.35">
       <c r="B9" t="s">
         <v>129</v>
       </c>
@@ -3905,8 +3984,11 @@
       <c r="K9">
         <v>1</v>
       </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L9">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.35">
       <c r="B10" t="s">
         <v>132</v>
       </c>
@@ -3937,8 +4019,11 @@
       <c r="K10">
         <v>3</v>
       </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L10">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.35">
       <c r="B11" t="s">
         <v>136</v>
       </c>
@@ -3969,8 +4054,11 @@
       <c r="K11">
         <v>2</v>
       </c>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L11">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.35">
       <c r="B12" t="s">
         <v>140</v>
       </c>
@@ -4001,8 +4089,11 @@
       <c r="K12">
         <v>4</v>
       </c>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L12">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.35">
       <c r="B13" t="s">
         <v>143</v>
       </c>
@@ -4033,8 +4124,11 @@
       <c r="K13">
         <v>2</v>
       </c>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L13">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.35">
       <c r="B14" t="s">
         <v>146</v>
       </c>
@@ -4065,8 +4159,11 @@
       <c r="K14">
         <v>3</v>
       </c>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L14">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.35">
       <c r="B15" t="s">
         <v>150</v>
       </c>
@@ -4097,8 +4194,11 @@
       <c r="K15">
         <v>4</v>
       </c>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L15">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.35">
       <c r="B16" t="s">
         <v>154</v>
       </c>
@@ -4128,6 +4228,9 @@
       </c>
       <c r="K16">
         <v>2</v>
+      </c>
+      <c r="L16">
+        <v>15</v>
       </c>
     </row>
   </sheetData>
@@ -4154,6 +4257,150 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{06A501E4-FC03-4FDC-BB80-55058995DF5C}">
+  <dimension ref="A1:B16"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B16" sqref="B16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="B14" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A15">
+        <v>14</v>
+      </c>
+      <c r="B15" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A16">
+        <v>15</v>
+      </c>
+      <c r="B16" t="s">
+        <v>995</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{33F95177-6FF6-4357-9D45-4774F681B352}">
   <dimension ref="A1:B5"/>
   <sheetViews>
@@ -4208,7 +4455,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D1C933FC-A45E-40A6-B8E6-F7E81A8E5430}">
   <dimension ref="A1:B71"/>
   <sheetViews>
@@ -4796,6 +5043,220 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{33D8DC69-2D44-47EA-901B-51D25516C119}">
+  <dimension ref="A1:D16"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="35.6328125" customWidth="1"/>
+    <col min="2" max="2" width="67.26953125" customWidth="1"/>
+    <col min="4" max="4" width="33.26953125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>997</v>
+      </c>
+      <c r="B1" t="s">
+        <v>998</v>
+      </c>
+      <c r="D1" t="s">
+        <v>998</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A2" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2" t="s">
+        <v>999</v>
+      </c>
+      <c r="D2">
+        <v>2948573948</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A3" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="B3" t="s">
+        <v>1000</v>
+      </c>
+      <c r="D3">
+        <v>5948304950</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A4" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="B4" t="s">
+        <v>1001</v>
+      </c>
+      <c r="D4">
+        <v>9482394394</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A5" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="B5" t="s">
+        <v>1002</v>
+      </c>
+      <c r="D5">
+        <v>4596803948</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A6" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="B6" t="s">
+        <v>1003</v>
+      </c>
+      <c r="D6">
+        <v>4950395604</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A7" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="B7" t="s">
+        <v>1004</v>
+      </c>
+      <c r="D7">
+        <v>9554450394</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A8" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="B8" t="s">
+        <v>1005</v>
+      </c>
+      <c r="D8">
+        <v>9334039405</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A9" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="B9" t="s">
+        <v>1006</v>
+      </c>
+      <c r="D9">
+        <v>9403940394</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A10" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="B10" t="s">
+        <v>1007</v>
+      </c>
+      <c r="D10">
+        <v>9409302930</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A11" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="B11" t="s">
+        <v>1008</v>
+      </c>
+      <c r="D11">
+        <v>9403904903</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A12" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="B12" t="s">
+        <v>1009</v>
+      </c>
+      <c r="D12">
+        <v>4950804930</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A13" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="B13" t="s">
+        <v>1010</v>
+      </c>
+      <c r="D13">
+        <v>9403904903</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A14" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="B14" t="s">
+        <v>1011</v>
+      </c>
+      <c r="D14">
+        <v>4954439504</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A15" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="B15" t="s">
+        <v>1012</v>
+      </c>
+      <c r="D15">
+        <v>2039049039</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A16" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="B16" t="s">
+        <v>1013</v>
+      </c>
+      <c r="D16">
+        <v>3459304950</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1" xr:uid="{EE0F6FB5-588A-45B7-A04D-5ED92C3F186C}"/>
+    <hyperlink ref="A3" r:id="rId2" xr:uid="{1C6B9478-49BB-4DFD-9E39-71B2F5DC5F9A}"/>
+    <hyperlink ref="A4" r:id="rId3" xr:uid="{9D68EB85-D9B5-4C62-9B30-CED06EFB66D3}"/>
+    <hyperlink ref="A5" r:id="rId4" xr:uid="{5A638817-6A5A-4537-B7D9-FBA102B87738}"/>
+    <hyperlink ref="A6" r:id="rId5" xr:uid="{8657DCA0-6CD8-4900-B0E8-F01696A8CC9C}"/>
+    <hyperlink ref="A7" r:id="rId6" xr:uid="{9E43C5FA-EC02-4B1A-8F47-A1F37C43B7DF}"/>
+    <hyperlink ref="A8" r:id="rId7" xr:uid="{02613C24-3C78-4E36-8276-45BFE0F4E3DC}"/>
+    <hyperlink ref="A9" r:id="rId8" xr:uid="{0E299C4A-9473-437A-83C7-BF9A9C63D86F}"/>
+    <hyperlink ref="A10" r:id="rId9" xr:uid="{90AADE60-0FC1-4BF5-A22A-76B2ACC480E3}"/>
+    <hyperlink ref="A11" r:id="rId10" xr:uid="{047C13D5-5E2D-4AC2-814B-561279FF5F7C}"/>
+    <hyperlink ref="A12" r:id="rId11" xr:uid="{E66740D1-B800-4FA4-B26E-44EEC9906464}"/>
+    <hyperlink ref="A13" r:id="rId12" xr:uid="{D0C04DC5-4F87-42D0-B5DB-F83D6959A50E}"/>
+    <hyperlink ref="A14" r:id="rId13" xr:uid="{35C16A05-5925-4AD7-BD7F-209CCD1D2AD6}"/>
+    <hyperlink ref="A15" r:id="rId14" xr:uid="{1ED87E61-79F9-40AC-8B38-87BFB31E3269}"/>
+    <hyperlink ref="A16" r:id="rId15" xr:uid="{9E30A28D-A3F3-4E28-8599-9C4B4CC27786}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="0" r:id="rId16"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{31E7C0C5-1485-4290-ADE2-68516D02BF10}">
   <dimension ref="A1:C16"/>
   <sheetViews>
@@ -4941,7 +5402,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EEC74DD5-0D89-49EA-9C01-9923BF1E41A0}">
   <dimension ref="B1:K226"/>
   <sheetViews>
@@ -12169,7 +12630,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EE303D13-90BC-4907-81A5-04C039D20B0F}">
   <dimension ref="B1:B16"/>
   <sheetViews>
@@ -12265,11 +12726,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C7835A59-A4F1-440E-9618-F4580ABF2227}">
   <dimension ref="B1:J271"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
@@ -16891,7 +17352,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D78006DC-90D4-44CD-B162-B0BF24BC0DCE}">
   <dimension ref="A1:B1"/>
   <sheetViews>
@@ -16914,7 +17375,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DFF660EC-2C0F-42D4-AADD-4A7EBE2ABEA1}">
   <dimension ref="B1:V106"/>
   <sheetViews>
@@ -19020,7 +19481,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A781D27D-40EE-46AF-BFFC-1D9AC12A4333}">
   <dimension ref="B1:B16"/>
   <sheetViews>
@@ -19113,148 +19574,4 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{06A501E4-FC03-4FDC-BB80-55058995DF5C}">
-  <dimension ref="A1:B16"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A2">
-        <v>1</v>
-      </c>
-      <c r="B2" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A3">
-        <v>2</v>
-      </c>
-      <c r="B3" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A4">
-        <v>3</v>
-      </c>
-      <c r="B4" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A5">
-        <v>4</v>
-      </c>
-      <c r="B5" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A6">
-        <v>5</v>
-      </c>
-      <c r="B6" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A7">
-        <v>6</v>
-      </c>
-      <c r="B7" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A8">
-        <v>7</v>
-      </c>
-      <c r="B8" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A9">
-        <v>8</v>
-      </c>
-      <c r="B9" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A10">
-        <v>9</v>
-      </c>
-      <c r="B10" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A11">
-        <v>10</v>
-      </c>
-      <c r="B11" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A12">
-        <v>11</v>
-      </c>
-      <c r="B12" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A13">
-        <v>12</v>
-      </c>
-      <c r="B13" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A14">
-        <v>13</v>
-      </c>
-      <c r="B14" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A15">
-        <v>14</v>
-      </c>
-      <c r="B15" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A16">
-        <v>15</v>
-      </c>
-      <c r="B16" t="s">
-        <v>995</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="0" r:id="rId1"/>
-</worksheet>
 </file>
</xml_diff>